<commit_message>
added ipad/desktop pikaday variations
</commit_message>
<xml_diff>
--- a/reporting/scoutapp/utils/Scouting-Report.xlsx
+++ b/reporting/scoutapp/utils/Scouting-Report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="208">
   <si>
     <t>Psyllid Scouting Report</t>
   </si>
@@ -170,7 +170,7 @@
     <t>Valencia</t>
   </si>
   <si>
-    <t>2017-02-23</t>
+    <t>2017-02-24</t>
   </si>
   <si>
     <t>X</t>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>102 A</t>
+  </si>
+  <si>
+    <t>2017-02-03</t>
   </si>
   <si>
     <t>102 B H</t>
@@ -288,6 +291,9 @@
   </si>
   <si>
     <t>N 81</t>
+  </si>
+  <si>
+    <t>2017-02-02</t>
   </si>
   <si>
     <t>QS</t>
@@ -530,6 +536,9 @@
     <t>Mixed</t>
   </si>
   <si>
+    <t>2017-01-16</t>
+  </si>
+  <si>
     <t>107 NRS West</t>
   </si>
   <si>
@@ -584,6 +593,12 @@
     <t>NW C 2</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
     <t>NW D 1</t>
   </si>
   <si>
@@ -618,6 +633,15 @@
   </si>
   <si>
     <t>120 D Young</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>low</t>
   </si>
 </sst>
 </file>
@@ -57920,26 +57944,110 @@
       <c r="D7" t="s">
         <v>50</v>
       </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4</v>
+      </c>
       <c r="I7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q7" t="n">
         <v>1</v>
       </c>
-      <c r="O7" t="n">
-        <v>1</v>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="W7" t="n">
+        <v>20</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>5</v>
       </c>
       <c r="AA7" t="n">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>51</v>
       </c>
       <c r="AG7" t="s">
         <v>51</v>
       </c>
+      <c r="AI7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>51</v>
+      </c>
       <c r="AM7" t="s">
         <v>51</v>
       </c>
+      <c r="AO7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>51</v>
+      </c>
       <c r="AS7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:45">
@@ -57949,21 +58057,192 @@
       <c r="B8" t="s">
         <v>49</v>
       </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:45">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
-        <v>55</v>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>3</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>6</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>51</v>
       </c>
       <c r="AS9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:45">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -57971,7 +58250,7 @@
     </row>
     <row r="11" spans="1:45">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -57979,7 +58258,7 @@
     </row>
     <row r="12" spans="1:45">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
@@ -57987,55 +58266,55 @@
     </row>
     <row r="13" spans="1:45">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:45">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:45">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:45">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:45">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:45">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:45">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
         <v>49</v>
@@ -58043,7 +58322,7 @@
     </row>
     <row r="20" spans="1:45">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
@@ -58051,71 +58330,71 @@
     </row>
     <row r="21" spans="1:45">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:45">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:45">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:45">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:45">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:45">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:45">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:45">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:45">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
@@ -58123,7 +58402,7 @@
     </row>
     <row r="30" spans="1:45">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
         <v>49</v>
@@ -58131,7 +58410,7 @@
     </row>
     <row r="31" spans="1:45">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
         <v>49</v>
@@ -58139,31 +58418,31 @@
     </row>
     <row r="32" spans="1:45">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:45">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:45">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:45">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
@@ -58171,15 +58450,15 @@
     </row>
     <row r="36" spans="1:45">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:45">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B37" t="s">
         <v>49</v>
@@ -58187,20 +58466,125 @@
     </row>
     <row r="38" spans="1:45">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:45">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:45">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" t="n">
+        <v>5</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3</v>
+      </c>
+      <c r="H40" t="n">
+        <v>4</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="n">
+        <v>0</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ40" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR40" t="s">
+        <v>51</v>
       </c>
       <c r="AS40" t="s">
         <v>51</v>
@@ -58208,7 +58592,7 @@
     </row>
     <row r="41" spans="1:45">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
         <v>49</v>
@@ -58216,7 +58600,7 @@
     </row>
     <row r="42" spans="1:45">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
@@ -58224,7 +58608,7 @@
     </row>
     <row r="43" spans="1:45">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
         <v>49</v>
@@ -58232,15 +58616,15 @@
     </row>
     <row r="44" spans="1:45">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:45">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B45" t="s">
         <v>49</v>
@@ -58248,15 +58632,15 @@
     </row>
     <row r="46" spans="1:45">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:45">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -58264,15 +58648,15 @@
     </row>
     <row r="48" spans="1:45">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:45">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
@@ -58280,15 +58664,15 @@
     </row>
     <row r="50" spans="1:45">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:45">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -58296,15 +58680,15 @@
     </row>
     <row r="52" spans="1:45">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:45">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
         <v>49</v>
@@ -58312,7 +58696,7 @@
     </row>
     <row r="54" spans="1:45">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B54" t="s">
         <v>49</v>
@@ -58320,15 +58704,15 @@
     </row>
     <row r="55" spans="1:45">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:45">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
         <v>49</v>
@@ -58336,7 +58720,7 @@
     </row>
     <row r="57" spans="1:45">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
         <v>49</v>
@@ -58344,23 +58728,23 @@
     </row>
     <row r="58" spans="1:45">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:45">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:45">
       <c r="A60" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s">
         <v>49</v>
@@ -58368,7 +58752,7 @@
     </row>
     <row r="61" spans="1:45">
       <c r="A61" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
         <v>49</v>
@@ -58376,15 +58760,15 @@
     </row>
     <row r="62" spans="1:45">
       <c r="A62" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:45">
       <c r="A63" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B63" t="s">
         <v>49</v>
@@ -58392,58 +58776,58 @@
     </row>
     <row r="64" spans="1:45">
       <c r="A64" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:45">
       <c r="A65" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:45">
       <c r="A66" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:45">
       <c r="A67" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:45">
       <c r="A68" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B68" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:45">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:45">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AS70" t="s">
         <v>51</v>
@@ -58451,7 +58835,7 @@
     </row>
     <row r="71" spans="1:45">
       <c r="A71" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B71" t="s">
         <v>49</v>
@@ -58459,15 +58843,15 @@
     </row>
     <row r="72" spans="1:45">
       <c r="A72" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:45">
       <c r="A73" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B73" t="s">
         <v>49</v>
@@ -58475,7 +58859,7 @@
     </row>
     <row r="74" spans="1:45">
       <c r="A74" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B74" t="s">
         <v>49</v>
@@ -58483,7 +58867,7 @@
     </row>
     <row r="75" spans="1:45">
       <c r="A75" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B75" t="s">
         <v>49</v>
@@ -58491,7 +58875,7 @@
     </row>
     <row r="76" spans="1:45">
       <c r="A76" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B76" t="s">
         <v>49</v>
@@ -58499,7 +58883,7 @@
     </row>
     <row r="77" spans="1:45">
       <c r="A77" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B77" t="s">
         <v>49</v>
@@ -58507,7 +58891,7 @@
     </row>
     <row r="78" spans="1:45">
       <c r="A78" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B78" t="s">
         <v>49</v>
@@ -58515,15 +58899,15 @@
     </row>
     <row r="79" spans="1:45">
       <c r="A79" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:45">
       <c r="A80" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B80" t="s">
         <v>49</v>
@@ -58531,23 +58915,23 @@
     </row>
     <row r="81" spans="1:45">
       <c r="A81" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B81" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:45">
       <c r="A82" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B82" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="1:45">
       <c r="A83" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B83" t="s">
         <v>49</v>
@@ -58555,23 +58939,23 @@
     </row>
     <row r="84" spans="1:45">
       <c r="A84" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B84" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:45">
       <c r="A85" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B85" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:45">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B86" t="s">
         <v>49</v>
@@ -58579,23 +58963,23 @@
     </row>
     <row r="87" spans="1:45">
       <c r="A87" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B87" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="88" spans="1:45">
       <c r="A88" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="89" spans="1:45">
       <c r="A89" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B89" t="s">
         <v>49</v>
@@ -58603,23 +58987,23 @@
     </row>
     <row r="90" spans="1:45">
       <c r="A90" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B90" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:45">
       <c r="A91" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B91" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:45">
       <c r="A92" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B92" t="s">
         <v>49</v>
@@ -58627,23 +59011,23 @@
     </row>
     <row r="93" spans="1:45">
       <c r="A93" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B93" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:45">
       <c r="A94" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B94" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" spans="1:45">
       <c r="A95" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B95" t="s">
         <v>49</v>
@@ -58651,7 +59035,7 @@
     </row>
     <row r="96" spans="1:45">
       <c r="A96" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B96" t="s">
         <v>49</v>
@@ -58659,15 +59043,15 @@
     </row>
     <row r="97" spans="1:45">
       <c r="A97" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B97" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="98" spans="1:45">
       <c r="A98" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B98" t="s">
         <v>49</v>
@@ -58675,15 +59059,15 @@
     </row>
     <row r="99" spans="1:45">
       <c r="A99" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:45">
       <c r="A100" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B100" t="s">
         <v>49</v>
@@ -58691,15 +59075,15 @@
     </row>
     <row r="101" spans="1:45">
       <c r="A101" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B101" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="102" spans="1:45">
       <c r="A102" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B102" t="s">
         <v>49</v>
@@ -58707,15 +59091,15 @@
     </row>
     <row r="103" spans="1:45">
       <c r="A103" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B103" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:45">
       <c r="A104" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B104" t="s">
         <v>49</v>
@@ -58723,7 +59107,7 @@
     </row>
     <row r="105" spans="1:45">
       <c r="A105" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B105" t="s">
         <v>49</v>
@@ -58731,31 +59115,31 @@
     </row>
     <row r="106" spans="1:45">
       <c r="A106" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B106" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:45">
       <c r="A107" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B107" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="108" spans="1:45">
       <c r="A108" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B108" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:45">
       <c r="A109" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B109" t="s">
         <v>49</v>
@@ -58763,50 +59147,71 @@
     </row>
     <row r="110" spans="1:45">
       <c r="A110" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B110" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="111" spans="1:45">
       <c r="A111" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B111" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112" spans="1:45">
       <c r="A112" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B112" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="113" spans="1:45">
       <c r="A113" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B113" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="114" spans="1:45">
       <c r="A114" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B114" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="1:45">
       <c r="A115" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B115" t="s">
-        <v>169</v>
+        <v>171</v>
+      </c>
+      <c r="D115" t="s">
+        <v>172</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0</v>
+      </c>
+      <c r="O115" t="n">
+        <v>0</v>
+      </c>
+      <c r="U115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG115" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM115" t="s">
+        <v>51</v>
       </c>
       <c r="AS115" t="s">
         <v>51</v>
@@ -58814,18 +59219,18 @@
     </row>
     <row r="116" spans="1:45">
       <c r="A116" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B116" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="117" spans="1:45">
       <c r="A117" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B117" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AS117" t="s">
         <v>51</v>
@@ -58833,7 +59238,7 @@
     </row>
     <row r="118" spans="1:45">
       <c r="A118" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B118" t="s">
         <v>49</v>
@@ -58844,10 +59249,10 @@
     </row>
     <row r="119" spans="1:45">
       <c r="A119" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B119" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AS119" t="s">
         <v>52</v>
@@ -58855,15 +59260,15 @@
     </row>
     <row r="120" spans="1:45">
       <c r="A120" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B120" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:45">
       <c r="A121" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B121" t="s">
         <v>49</v>
@@ -58871,7 +59276,7 @@
     </row>
     <row r="122" spans="1:45">
       <c r="A122" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B122" t="s">
         <v>49</v>
@@ -58879,7 +59284,7 @@
     </row>
     <row r="123" spans="1:45">
       <c r="A123" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B123" t="s">
         <v>49</v>
@@ -58887,18 +59292,18 @@
     </row>
     <row r="124" spans="1:45">
       <c r="A124" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B124" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="1:45">
       <c r="A125" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B125" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -58962,7 +59367,7 @@
       </c>
       <c r="C2" s="39" t="n"/>
       <c r="G2" s="19" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="J2" s="19" t="n"/>
       <c r="L2" s="19" t="n"/>
@@ -58974,7 +59379,7 @@
       <c r="O2" s="19" t="n"/>
       <c r="P2" s="19" t="n"/>
       <c r="Q2" s="19" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="R2" s="19" t="n"/>
       <c r="S2" s="19" t="n"/>
@@ -58989,7 +59394,7 @@
     </row>
     <row r="4" spans="1:39">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:39">
@@ -59003,13 +59408,13 @@
         <v>30</v>
       </c>
       <c r="W6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="AC6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="AI6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:39">
@@ -59118,23 +59523,116 @@
     </row>
     <row r="8" spans="1:39">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
       </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>192</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>192</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>192</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>192</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="9" spans="1:39">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:39">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -59142,15 +59640,15 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:39">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
@@ -59158,15 +59656,15 @@
     </row>
     <row r="13" spans="1:39">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:39">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
@@ -59174,15 +59672,15 @@
     </row>
     <row r="15" spans="1:39">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:39">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
@@ -59190,15 +59688,15 @@
     </row>
     <row r="17" spans="1:39">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:39">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
         <v>49</v>
@@ -59206,12 +59704,105 @@
     </row>
     <row r="19" spans="1:39">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:39">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>204</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>5</v>
+      </c>
+      <c r="K20" t="n">
+        <v>9</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>1</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>191</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>191</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>205</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>206</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>192</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>206</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>